<commit_message>
Created first graph on pbix
</commit_message>
<xml_diff>
--- a/data/Staff per team.xlsx
+++ b/data/Staff per team.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="780" documentId="14_{7ECA4B77-9B9E-44F7-8F2C-46443369A0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EADBDBDB-F841-4571-B4C4-654C6620B3E9}"/>
+  <xr:revisionPtr revIDLastSave="816" documentId="14_{7ECA4B77-9B9E-44F7-8F2C-46443369A0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5BE53ED-B082-4E94-8C1D-7B533D883159}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
+    <workbookView xWindow="10245" yWindow="3375" windowWidth="14805" windowHeight="7785" activeTab="3" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
   </bookViews>
   <sheets>
     <sheet name="All roles per team" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6125" uniqueCount="2451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6156" uniqueCount="2482">
   <si>
     <t>Name</t>
   </si>
@@ -7387,6 +7387,99 @@
   </si>
   <si>
     <t>Jack Hanley</t>
+  </si>
+  <si>
+    <t>ARI</t>
+  </si>
+  <si>
+    <t>Team-city</t>
+  </si>
+  <si>
+    <t>LAA</t>
+  </si>
+  <si>
+    <t>BAL</t>
+  </si>
+  <si>
+    <t>BOS</t>
+  </si>
+  <si>
+    <t>CHC</t>
+  </si>
+  <si>
+    <t>CHW</t>
+  </si>
+  <si>
+    <t>CIN</t>
+  </si>
+  <si>
+    <t>CLE</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t>HOU</t>
+  </si>
+  <si>
+    <t>OAK</t>
+  </si>
+  <si>
+    <t>TOR</t>
+  </si>
+  <si>
+    <t>ATL</t>
+  </si>
+  <si>
+    <t>MIL</t>
+  </si>
+  <si>
+    <t>STL</t>
+  </si>
+  <si>
+    <t>LAD</t>
+  </si>
+  <si>
+    <t>SFG</t>
+  </si>
+  <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>MIA</t>
+  </si>
+  <si>
+    <t>NYM</t>
+  </si>
+  <si>
+    <t>WSN</t>
+  </si>
+  <si>
+    <t>SDP</t>
+  </si>
+  <si>
+    <t>PHI</t>
+  </si>
+  <si>
+    <t>PIT</t>
+  </si>
+  <si>
+    <t>TEX</t>
+  </si>
+  <si>
+    <t>TBR</t>
+  </si>
+  <si>
+    <t>KCR</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>NYY</t>
   </si>
 </sst>
 </file>
@@ -7451,1165 +7544,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="298">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="103">
     <dxf>
       <fill>
         <patternFill>
@@ -9012,6 +7955,41 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -9200,271 +8178,91 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -9538,89 +8336,11 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="1"/>
         </top>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -9653,28 +8373,22 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCE4D6"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -9701,7 +8415,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{40A49B79-4F51-4334-A76E-80677356E5C0}" name="Table5" displayName="Table5" ref="A1:C1495" totalsRowShown="0">
   <autoFilter ref="A1:C1495" xr:uid="{40A49B79-4F51-4334-A76E-80677356E5C0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C1495">
-    <sortCondition sortBy="cellColor" ref="A1:A1495" dxfId="44"/>
+    <sortCondition sortBy="cellColor" ref="A1:A1495" dxfId="102"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{BB65CBB8-4BCF-43D2-B3A7-6A54553A1BAC}" name="Position"/>
@@ -9727,29 +8441,30 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DD3EF1CA-61C6-4F74-BDD0-906E5460B1EE}" name="Table3" displayName="Table3" ref="A1:C504" totalsRowShown="0" headerRowDxfId="286" dataDxfId="0" headerRowBorderDxfId="287" tableBorderDxfId="288">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DD3EF1CA-61C6-4F74-BDD0-906E5460B1EE}" name="Table3" displayName="Table3" ref="A1:C504" totalsRowShown="0" headerRowDxfId="101" dataDxfId="99" headerRowBorderDxfId="100" tableBorderDxfId="98">
   <autoFilter ref="A1:C504" xr:uid="{DD3EF1CA-61C6-4F74-BDD0-906E5460B1EE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C504">
     <sortCondition ref="C1:C504"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{63937850-0C8D-487C-8427-DFC70DF590F0}" name="Position" dataDxfId="285"/>
-    <tableColumn id="2" xr3:uid="{49901D13-E91B-4EE6-9756-20B7F605DDA8}" name="Name" dataDxfId="284"/>
-    <tableColumn id="3" xr3:uid="{D9299361-C6F7-4992-B1D8-9ECD277BF085}" name="Team" dataDxfId="283"/>
+    <tableColumn id="1" xr3:uid="{63937850-0C8D-487C-8427-DFC70DF590F0}" name="Position" dataDxfId="97"/>
+    <tableColumn id="2" xr3:uid="{49901D13-E91B-4EE6-9756-20B7F605DDA8}" name="Name" dataDxfId="96"/>
+    <tableColumn id="3" xr3:uid="{D9299361-C6F7-4992-B1D8-9ECD277BF085}" name="Team" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73E95DFB-2414-42BF-8D4F-BDFF95454085}" name="Table1" displayName="Table1" ref="A1:B31" totalsRowShown="0" headerRowDxfId="291" dataDxfId="290" tableBorderDxfId="293">
-  <autoFilter ref="A1:B31" xr:uid="{73E95DFB-2414-42BF-8D4F-BDFF95454085}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B31">
-    <sortCondition ref="B1:B31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73E95DFB-2414-42BF-8D4F-BDFF95454085}" name="Table1" displayName="Table1" ref="A1:C31" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93" tableBorderDxfId="92">
+  <autoFilter ref="A1:C31" xr:uid="{73E95DFB-2414-42BF-8D4F-BDFF95454085}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C31">
+    <sortCondition ref="C1:C31"/>
   </sortState>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{BB93A38C-3D1F-4EBA-9347-B1AE82A135ED}" name="Team" dataDxfId="292"/>
-    <tableColumn id="2" xr3:uid="{094F86E6-DE94-49CA-9ACE-DFDA362DE830}" name="Size" dataDxfId="289"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{BB93A38C-3D1F-4EBA-9347-B1AE82A135ED}" name="Team" dataDxfId="91"/>
+    <tableColumn id="3" xr3:uid="{A62A3568-6650-4680-9CDB-CBAD667955AF}" name="Team-city"/>
+    <tableColumn id="2" xr3:uid="{094F86E6-DE94-49CA-9ACE-DFDA362DE830}" name="Size" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -26514,7 +25229,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A5:A6">
-    <cfRule type="containsText" dxfId="204" priority="42" operator="containsText" text="Research">
+    <cfRule type="containsText" dxfId="89" priority="42" operator="containsText" text="Research">
       <formula>NOT(ISERROR(SEARCH("Research",A5)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="43" operator="containsText" text="Research">
@@ -26522,131 +25237,131 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="120" priority="36" operator="containsText" text="Data Engineer">
+    <cfRule type="containsText" dxfId="88" priority="36" operator="containsText" text="Data Engineer">
       <formula>NOT(ISERROR(SEARCH("Data Engineer",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="37" operator="containsText" text="Quantitative Analysis">
+    <cfRule type="containsText" dxfId="87" priority="37" operator="containsText" text="Quantitative Analysis">
       <formula>NOT(ISERROR(SEARCH("Quantitative Analysis",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="38" operator="containsText" text="Research Scientist">
+    <cfRule type="containsText" dxfId="86" priority="38" operator="containsText" text="Research Scientist">
       <formula>NOT(ISERROR(SEARCH("Research Scientist",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="39" operator="containsText" text="Research &amp; Analytics">
+    <cfRule type="containsText" dxfId="85" priority="39" operator="containsText" text="Research &amp; Analytics">
       <formula>NOT(ISERROR(SEARCH("Research &amp; Analytics",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="40" operator="containsText" text="Research &amp; Development">
+    <cfRule type="containsText" dxfId="84" priority="40" operator="containsText" text="Research &amp; Development">
       <formula>NOT(ISERROR(SEARCH("Research &amp; Development",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="41" operator="containsText" text="Research">
+    <cfRule type="containsText" dxfId="83" priority="41" operator="containsText" text="Research">
       <formula>NOT(ISERROR(SEARCH("Research",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A1495">
-    <cfRule type="containsText" dxfId="114" priority="1" operator="containsText" text="Assistant">
+    <cfRule type="containsText" dxfId="82" priority="1" operator="containsText" text="Assistant">
       <formula>NOT(ISERROR(SEARCH("Assistant",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="2" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="81" priority="2" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="3" operator="containsText" text="Analytics">
+    <cfRule type="containsText" dxfId="80" priority="3" operator="containsText" text="Analytics">
       <formula>NOT(ISERROR(SEARCH("Analytics",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="4" operator="containsText" text="Business Development &amp; Analytics">
+    <cfRule type="containsText" dxfId="79" priority="4" operator="containsText" text="Business Development &amp; Analytics">
       <formula>NOT(ISERROR(SEARCH("Business Development &amp; Analytics",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="5" operator="containsText" text="Data Operations">
+    <cfRule type="containsText" dxfId="78" priority="5" operator="containsText" text="Data Operations">
       <formula>NOT(ISERROR(SEARCH("Data Operations",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="6" operator="containsText" text="Database">
+    <cfRule type="containsText" dxfId="77" priority="6" operator="containsText" text="Database">
       <formula>NOT(ISERROR(SEARCH("Database",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="7" operator="containsText" text="Software Developer">
+    <cfRule type="containsText" dxfId="76" priority="7" operator="containsText" text="Software Developer">
       <formula>NOT(ISERROR(SEARCH("Software Developer",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="8" operator="containsText" text="Software Engineer">
+    <cfRule type="containsText" dxfId="75" priority="8" operator="containsText" text="Software Engineer">
       <formula>NOT(ISERROR(SEARCH("Software Engineer",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="9" operator="containsText" text="Strategies">
+    <cfRule type="containsText" dxfId="74" priority="9" operator="containsText" text="Strategies">
       <formula>NOT(ISERROR(SEARCH("Strategies",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="10" operator="containsText" text="Baseball Operations – Systems">
+    <cfRule type="containsText" dxfId="73" priority="10" operator="containsText" text="Baseball Operations – Systems">
       <formula>NOT(ISERROR(SEARCH("Baseball Operations – Systems",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="11" operator="containsText" text="Analyst">
+    <cfRule type="containsText" dxfId="72" priority="11" operator="containsText" text="Analyst">
       <formula>NOT(ISERROR(SEARCH("Analyst",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="12" operator="containsText" text=" Baseball Developmental Technology">
+    <cfRule type="containsText" dxfId="71" priority="12" operator="containsText" text=" Baseball Developmental Technology">
       <formula>NOT(ISERROR(SEARCH(" Baseball Developmental Technology",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="13" operator="containsText" text="Player Development">
+    <cfRule type="containsText" dxfId="70" priority="13" operator="containsText" text="Player Development">
       <formula>NOT(ISERROR(SEARCH("Player Development",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="14" operator="containsText" text="Pro Analytics">
+    <cfRule type="containsText" dxfId="69" priority="14" operator="containsText" text="Pro Analytics">
       <formula>NOT(ISERROR(SEARCH("Pro Analytics",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="15" operator="containsText" text="Business Intelligience Analyst">
+    <cfRule type="containsText" dxfId="68" priority="15" operator="containsText" text="Business Intelligience Analyst">
       <formula>NOT(ISERROR(SEARCH("Business Intelligience Analyst",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="16" operator="containsText" text="Business Analyst">
+    <cfRule type="containsText" dxfId="67" priority="16" operator="containsText" text="Business Analyst">
       <formula>NOT(ISERROR(SEARCH("Business Analyst",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="17" operator="containsText" text="Baseball Systems">
+    <cfRule type="containsText" dxfId="66" priority="17" operator="containsText" text="Baseball Systems">
       <formula>NOT(ISERROR(SEARCH("Baseball Systems",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="18" operator="containsText" text="R&amp;D">
+    <cfRule type="containsText" dxfId="65" priority="18" operator="containsText" text="R&amp;D">
       <formula>NOT(ISERROR(SEARCH("R&amp;D",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="19" operator="containsText" text="Pitching Analytics">
+    <cfRule type="containsText" dxfId="64" priority="19" operator="containsText" text="Pitching Analytics">
       <formula>NOT(ISERROR(SEARCH("Pitching Analytics",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="20" operator="containsText" text="Pitching Strategist">
+    <cfRule type="containsText" dxfId="63" priority="20" operator="containsText" text="Pitching Strategist">
       <formula>NOT(ISERROR(SEARCH("Pitching Strategist",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="21" operator="containsText" text="Assistant">
+    <cfRule type="containsText" dxfId="62" priority="21" operator="containsText" text="Assistant">
       <formula>NOT(ISERROR(SEARCH("Assistant",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="23" operator="containsText" text="Baseball Operations Fellow">
+    <cfRule type="containsText" dxfId="61" priority="23" operator="containsText" text="Baseball Operations Fellow">
       <formula>NOT(ISERROR(SEARCH("Baseball Operations Fellow",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="24" operator="containsText" text="Baseball Operations Analyst">
+    <cfRule type="containsText" dxfId="60" priority="24" operator="containsText" text="Baseball Operations Analyst">
       <formula>NOT(ISERROR(SEARCH("Baseball Operations Analyst",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="25" operator="containsText" text="Strategy">
+    <cfRule type="containsText" dxfId="59" priority="25" operator="containsText" text="Strategy">
       <formula>NOT(ISERROR(SEARCH("Strategy",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="26" operator="containsText" text="Business Strategy">
+    <cfRule type="containsText" dxfId="58" priority="26" operator="containsText" text="Business Strategy">
       <formula>NOT(ISERROR(SEARCH("Business Strategy",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="27" operator="containsText" text="Baseball Analytics">
+    <cfRule type="containsText" dxfId="57" priority="27" operator="containsText" text="Baseball Analytics">
       <formula>NOT(ISERROR(SEARCH("Baseball Analytics",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="28" operator="containsText" text="Business Analytics">
+    <cfRule type="containsText" dxfId="56" priority="28" operator="containsText" text="Business Analytics">
       <formula>NOT(ISERROR(SEARCH("Business Analytics",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="29" operator="containsText" text="Business Insights">
+    <cfRule type="containsText" dxfId="55" priority="29" operator="containsText" text="Business Insights">
       <formula>NOT(ISERROR(SEARCH("Business Insights",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="30" operator="containsText" text="Business Intelligence">
+    <cfRule type="containsText" dxfId="54" priority="30" operator="containsText" text="Business Intelligence">
       <formula>NOT(ISERROR(SEARCH("Business Intelligence",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="31" operator="containsText" text="Baseball System Developer">
+    <cfRule type="containsText" dxfId="53" priority="31" operator="containsText" text="Baseball System Developer">
       <formula>NOT(ISERROR(SEARCH("Baseball System Developer",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="32" operator="containsText" text="Software Engineer">
+    <cfRule type="containsText" dxfId="52" priority="32" operator="containsText" text="Software Engineer">
       <formula>NOT(ISERROR(SEARCH("Software Engineer",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="33" operator="containsText" text="DevOps">
+    <cfRule type="containsText" dxfId="51" priority="33" operator="containsText" text="DevOps">
       <formula>NOT(ISERROR(SEARCH("DevOps",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="34" operator="containsText" text="Data Quality Assurance">
+    <cfRule type="containsText" dxfId="50" priority="34" operator="containsText" text="Data Quality Assurance">
       <formula>NOT(ISERROR(SEARCH("Data Quality Assurance",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="35" operator="containsText" text="Data Scientist">
+    <cfRule type="containsText" dxfId="49" priority="35" operator="containsText" text="Data Scientist">
       <formula>NOT(ISERROR(SEARCH("Data Scientist",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A328">
-    <cfRule type="containsText" dxfId="203" priority="22" operator="containsText" text="Player Development">
+    <cfRule type="containsText" dxfId="48" priority="22" operator="containsText" text="Player Development">
       <formula>NOT(ISERROR(SEARCH("Player Development",A328)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27127,13 +25842,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>1948</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -32672,27 +31387,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="containsText" dxfId="201" priority="119" operator="containsText" text="Data Engineer">
+    <cfRule type="containsText" dxfId="47" priority="119" operator="containsText" text="Data Engineer">
       <formula>NOT(ISERROR(SEARCH("Data Engineer",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="200" priority="120" operator="containsText" text="Quantitative Analysis">
+    <cfRule type="containsText" dxfId="46" priority="120" operator="containsText" text="Quantitative Analysis">
       <formula>NOT(ISERROR(SEARCH("Quantitative Analysis",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="199" priority="121" operator="containsText" text="Research Scientist">
+    <cfRule type="containsText" dxfId="45" priority="121" operator="containsText" text="Research Scientist">
       <formula>NOT(ISERROR(SEARCH("Research Scientist",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="122" operator="containsText" text="Research &amp; Analytics">
+    <cfRule type="containsText" dxfId="44" priority="122" operator="containsText" text="Research &amp; Analytics">
       <formula>NOT(ISERROR(SEARCH("Research &amp; Analytics",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="197" priority="123" operator="containsText" text="Research &amp; Development">
+    <cfRule type="containsText" dxfId="43" priority="123" operator="containsText" text="Research &amp; Development">
       <formula>NOT(ISERROR(SEARCH("Research &amp; Development",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="196" priority="124" operator="containsText" text="Research">
+    <cfRule type="containsText" dxfId="42" priority="124" operator="containsText" text="Research">
       <formula>NOT(ISERROR(SEARCH("Research",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:A7">
-    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="Research">
+    <cfRule type="containsText" dxfId="41" priority="42" operator="containsText" text="Research">
       <formula>NOT(ISERROR(SEARCH("Research",A6)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="43" operator="containsText" text="Research">
@@ -32700,131 +31415,131 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A504">
-    <cfRule type="containsText" dxfId="41" priority="36" operator="containsText" text="Data Engineer">
+    <cfRule type="containsText" dxfId="40" priority="36" operator="containsText" text="Data Engineer">
       <formula>NOT(ISERROR(SEARCH("Data Engineer",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="37" operator="containsText" text="Quantitative Analysis">
+    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="Quantitative Analysis">
       <formula>NOT(ISERROR(SEARCH("Quantitative Analysis",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="38" operator="containsText" text="Research Scientist">
+    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="Research Scientist">
       <formula>NOT(ISERROR(SEARCH("Research Scientist",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="39" operator="containsText" text="Research &amp; Analytics">
+    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="Research &amp; Analytics">
       <formula>NOT(ISERROR(SEARCH("Research &amp; Analytics",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="40" operator="containsText" text="Research &amp; Development">
+    <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="Research &amp; Development">
       <formula>NOT(ISERROR(SEARCH("Research &amp; Development",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="41" operator="containsText" text="Research">
+    <cfRule type="containsText" dxfId="35" priority="41" operator="containsText" text="Research">
       <formula>NOT(ISERROR(SEARCH("Research",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A504">
-    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="Assistant">
+    <cfRule type="containsText" dxfId="34" priority="1" operator="containsText" text="Assistant">
       <formula>NOT(ISERROR(SEARCH("Assistant",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="33" priority="2" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="Analytics">
+    <cfRule type="containsText" dxfId="32" priority="3" operator="containsText" text="Analytics">
       <formula>NOT(ISERROR(SEARCH("Analytics",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="Business Development &amp; Analytics">
+    <cfRule type="containsText" dxfId="31" priority="4" operator="containsText" text="Business Development &amp; Analytics">
       <formula>NOT(ISERROR(SEARCH("Business Development &amp; Analytics",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="Data Operations">
+    <cfRule type="containsText" dxfId="30" priority="5" operator="containsText" text="Data Operations">
       <formula>NOT(ISERROR(SEARCH("Data Operations",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="6" operator="containsText" text="Database">
+    <cfRule type="containsText" dxfId="29" priority="6" operator="containsText" text="Database">
       <formula>NOT(ISERROR(SEARCH("Database",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="7" operator="containsText" text="Software Developer">
+    <cfRule type="containsText" dxfId="28" priority="7" operator="containsText" text="Software Developer">
       <formula>NOT(ISERROR(SEARCH("Software Developer",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="8" operator="containsText" text="Software Engineer">
+    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Software Engineer">
       <formula>NOT(ISERROR(SEARCH("Software Engineer",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="Strategies">
+    <cfRule type="containsText" dxfId="26" priority="9" operator="containsText" text="Strategies">
       <formula>NOT(ISERROR(SEARCH("Strategies",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="10" operator="containsText" text="Baseball Operations – Systems">
+    <cfRule type="containsText" dxfId="25" priority="10" operator="containsText" text="Baseball Operations – Systems">
       <formula>NOT(ISERROR(SEARCH("Baseball Operations – Systems",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="11" operator="containsText" text="Analyst">
+    <cfRule type="containsText" dxfId="24" priority="11" operator="containsText" text="Analyst">
       <formula>NOT(ISERROR(SEARCH("Analyst",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="12" operator="containsText" text=" Baseball Developmental Technology">
+    <cfRule type="containsText" dxfId="23" priority="12" operator="containsText" text=" Baseball Developmental Technology">
       <formula>NOT(ISERROR(SEARCH(" Baseball Developmental Technology",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="Player Development">
+    <cfRule type="containsText" dxfId="22" priority="13" operator="containsText" text="Player Development">
       <formula>NOT(ISERROR(SEARCH("Player Development",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="Pro Analytics">
+    <cfRule type="containsText" dxfId="21" priority="14" operator="containsText" text="Pro Analytics">
       <formula>NOT(ISERROR(SEARCH("Pro Analytics",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="Business Intelligience Analyst">
+    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="Business Intelligience Analyst">
       <formula>NOT(ISERROR(SEARCH("Business Intelligience Analyst",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Business Analyst">
+    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="Business Analyst">
       <formula>NOT(ISERROR(SEARCH("Business Analyst",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Baseball Systems">
+    <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="Baseball Systems">
       <formula>NOT(ISERROR(SEARCH("Baseball Systems",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="R&amp;D">
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="R&amp;D">
       <formula>NOT(ISERROR(SEARCH("R&amp;D",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Pitching Analytics">
+    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="Pitching Analytics">
       <formula>NOT(ISERROR(SEARCH("Pitching Analytics",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="Pitching Strategist">
+    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="Pitching Strategist">
       <formula>NOT(ISERROR(SEARCH("Pitching Strategist",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="Assistant">
+    <cfRule type="containsText" dxfId="14" priority="21" operator="containsText" text="Assistant">
       <formula>NOT(ISERROR(SEARCH("Assistant",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="23" operator="containsText" text="Baseball Operations Fellow">
+    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="Baseball Operations Fellow">
       <formula>NOT(ISERROR(SEARCH("Baseball Operations Fellow",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="24" operator="containsText" text="Baseball Operations Analyst">
+    <cfRule type="containsText" dxfId="12" priority="24" operator="containsText" text="Baseball Operations Analyst">
       <formula>NOT(ISERROR(SEARCH("Baseball Operations Analyst",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="25" operator="containsText" text="Strategy">
+    <cfRule type="containsText" dxfId="11" priority="25" operator="containsText" text="Strategy">
       <formula>NOT(ISERROR(SEARCH("Strategy",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="26" operator="containsText" text="Business Strategy">
+    <cfRule type="containsText" dxfId="10" priority="26" operator="containsText" text="Business Strategy">
       <formula>NOT(ISERROR(SEARCH("Business Strategy",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="27" operator="containsText" text="Baseball Analytics">
+    <cfRule type="containsText" dxfId="9" priority="27" operator="containsText" text="Baseball Analytics">
       <formula>NOT(ISERROR(SEARCH("Baseball Analytics",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="28" operator="containsText" text="Business Analytics">
+    <cfRule type="containsText" dxfId="8" priority="28" operator="containsText" text="Business Analytics">
       <formula>NOT(ISERROR(SEARCH("Business Analytics",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="29" operator="containsText" text="Business Insights">
+    <cfRule type="containsText" dxfId="7" priority="29" operator="containsText" text="Business Insights">
       <formula>NOT(ISERROR(SEARCH("Business Insights",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="30" operator="containsText" text="Business Intelligence">
+    <cfRule type="containsText" dxfId="6" priority="30" operator="containsText" text="Business Intelligence">
       <formula>NOT(ISERROR(SEARCH("Business Intelligence",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="31" operator="containsText" text="Baseball System Developer">
+    <cfRule type="containsText" dxfId="5" priority="31" operator="containsText" text="Baseball System Developer">
       <formula>NOT(ISERROR(SEARCH("Baseball System Developer",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="32" operator="containsText" text="Software Engineer">
+    <cfRule type="containsText" dxfId="4" priority="32" operator="containsText" text="Software Engineer">
       <formula>NOT(ISERROR(SEARCH("Software Engineer",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="33" operator="containsText" text="DevOps">
+    <cfRule type="containsText" dxfId="3" priority="33" operator="containsText" text="DevOps">
       <formula>NOT(ISERROR(SEARCH("DevOps",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="34" operator="containsText" text="Data Quality Assurance">
+    <cfRule type="containsText" dxfId="2" priority="34" operator="containsText" text="Data Quality Assurance">
       <formula>NOT(ISERROR(SEARCH("Data Quality Assurance",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="35" operator="containsText" text="Data Scientist">
+    <cfRule type="containsText" dxfId="1" priority="35" operator="containsText" text="Data Scientist">
       <formula>NOT(ISERROR(SEARCH("Data Scientist",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A329">
-    <cfRule type="containsText" dxfId="1" priority="22" operator="containsText" text="Player Development">
+    <cfRule type="containsText" dxfId="0" priority="22" operator="containsText" text="Player Development">
       <formula>NOT(ISERROR(SEARCH("Player Development",A329)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32844,262 +31559,356 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D476075A-8E69-4DC1-BFAB-B7691E10E09E}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>2452</v>
+      </c>
+      <c r="C1" t="s">
         <v>2364</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>716</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C2">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>431</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" t="s">
+        <v>2458</v>
+      </c>
+      <c r="C3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>472</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" t="s">
+        <v>2460</v>
+      </c>
+      <c r="C4">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>1045</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" t="s">
+        <v>2462</v>
+      </c>
+      <c r="C5">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>1799</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" t="s">
+        <v>2463</v>
+      </c>
+      <c r="C6">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>1305</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" t="s">
+        <v>2475</v>
+      </c>
+      <c r="C7">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>1800</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" t="s">
+        <v>2472</v>
+      </c>
+      <c r="C8">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>332</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" t="s">
+        <v>2454</v>
+      </c>
+      <c r="C9">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>256</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" t="s">
+        <v>2464</v>
+      </c>
+      <c r="C10">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>1497</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" t="s">
+        <v>2466</v>
+      </c>
+      <c r="C11">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>573</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" t="s">
+        <v>2478</v>
+      </c>
+      <c r="C12">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>1331</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" t="s">
+        <v>2473</v>
+      </c>
+      <c r="C13">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>1741</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" t="s">
+        <v>2476</v>
+      </c>
+      <c r="C14">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>390</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" t="s">
+        <v>2457</v>
+      </c>
+      <c r="C15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>1457</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" t="s">
+        <v>2469</v>
+      </c>
+      <c r="C16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>474</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" t="s">
+        <v>2479</v>
+      </c>
+      <c r="C17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>635</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" t="s">
+        <v>2453</v>
+      </c>
+      <c r="C18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>797</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" t="s">
+        <v>2465</v>
+      </c>
+      <c r="C19">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>374</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" t="s">
+        <v>2456</v>
+      </c>
+      <c r="C20">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>798</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" t="s">
+        <v>2480</v>
+      </c>
+      <c r="C21">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>963</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" t="s">
+        <v>2481</v>
+      </c>
+      <c r="C22">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>482</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" t="s">
+        <v>2461</v>
+      </c>
+      <c r="C23">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>455</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" t="s">
+        <v>2459</v>
+      </c>
+      <c r="C24">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" t="s">
+        <v>2451</v>
+      </c>
+      <c r="C25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>879</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" t="s">
+        <v>2471</v>
+      </c>
+      <c r="C26">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>1333</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" t="s">
+        <v>2468</v>
+      </c>
+      <c r="C27">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>345</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" t="s">
+        <v>2455</v>
+      </c>
+      <c r="C28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>1125</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" t="s">
+        <v>2474</v>
+      </c>
+      <c r="C29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>702</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" t="s">
+        <v>2467</v>
+      </c>
+      <c r="C30">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>1682</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" t="s">
+        <v>2477</v>
+      </c>
+      <c r="C31">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created Analytical staff vs all pitchers signed stats file
</commit_message>
<xml_diff>
--- a/data/Staff per team.xlsx
+++ b/data/Staff per team.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="816" documentId="14_{7ECA4B77-9B9E-44F7-8F2C-46443369A0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5BE53ED-B082-4E94-8C1D-7B533D883159}"/>
+  <xr:revisionPtr revIDLastSave="817" documentId="14_{7ECA4B77-9B9E-44F7-8F2C-46443369A0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DECFCE1-C936-4ABA-A340-66813FF13238}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="3375" windowWidth="14805" windowHeight="7785" activeTab="3" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
+    <workbookView xWindow="9540" yWindow="16380" windowWidth="14805" windowHeight="7785" activeTab="3" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
   </bookViews>
   <sheets>
     <sheet name="All roles per team" sheetId="1" r:id="rId1"/>
@@ -7553,6 +7553,213 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="103">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -7891,6 +8098,14 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2EFDA"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
@@ -8183,221 +8398,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE2EFDA"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -8411,11 +8411,15 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{40A49B79-4F51-4334-A76E-80677356E5C0}" name="Table5" displayName="Table5" ref="A1:C1495" totalsRowShown="0">
   <autoFilter ref="A1:C1495" xr:uid="{40A49B79-4F51-4334-A76E-80677356E5C0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C1495">
-    <sortCondition sortBy="cellColor" ref="A1:A1495" dxfId="102"/>
+    <sortCondition sortBy="cellColor" ref="A1:A1495" dxfId="60"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{BB65CBB8-4BCF-43D2-B3A7-6A54553A1BAC}" name="Position"/>
@@ -8441,30 +8445,30 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DD3EF1CA-61C6-4F74-BDD0-906E5460B1EE}" name="Table3" displayName="Table3" ref="A1:C504" totalsRowShown="0" headerRowDxfId="101" dataDxfId="99" headerRowBorderDxfId="100" tableBorderDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DD3EF1CA-61C6-4F74-BDD0-906E5460B1EE}" name="Table3" displayName="Table3" ref="A1:C504" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
   <autoFilter ref="A1:C504" xr:uid="{DD3EF1CA-61C6-4F74-BDD0-906E5460B1EE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C504">
     <sortCondition ref="C1:C504"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{63937850-0C8D-487C-8427-DFC70DF590F0}" name="Position" dataDxfId="97"/>
-    <tableColumn id="2" xr3:uid="{49901D13-E91B-4EE6-9756-20B7F605DDA8}" name="Name" dataDxfId="96"/>
-    <tableColumn id="3" xr3:uid="{D9299361-C6F7-4992-B1D8-9ECD277BF085}" name="Team" dataDxfId="95"/>
+    <tableColumn id="1" xr3:uid="{63937850-0C8D-487C-8427-DFC70DF590F0}" name="Position" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{49901D13-E91B-4EE6-9756-20B7F605DDA8}" name="Name" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{D9299361-C6F7-4992-B1D8-9ECD277BF085}" name="Team" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73E95DFB-2414-42BF-8D4F-BDFF95454085}" name="Table1" displayName="Table1" ref="A1:C31" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93" tableBorderDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73E95DFB-2414-42BF-8D4F-BDFF95454085}" name="Table1" displayName="Table1" ref="A1:C31" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="A1:C31" xr:uid="{73E95DFB-2414-42BF-8D4F-BDFF95454085}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C31">
-    <sortCondition ref="C1:C31"/>
+    <sortCondition descending="1" ref="C1:C31"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{BB93A38C-3D1F-4EBA-9347-B1AE82A135ED}" name="Team" dataDxfId="91"/>
+    <tableColumn id="1" xr3:uid="{BB93A38C-3D1F-4EBA-9347-B1AE82A135ED}" name="Team" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{A62A3568-6650-4680-9CDB-CBAD667955AF}" name="Team-city"/>
-    <tableColumn id="2" xr3:uid="{094F86E6-DE94-49CA-9ACE-DFDA362DE830}" name="Size" dataDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{094F86E6-DE94-49CA-9ACE-DFDA362DE830}" name="Size" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -25229,7 +25233,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A5:A6">
-    <cfRule type="containsText" dxfId="89" priority="42" operator="containsText" text="Research">
+    <cfRule type="containsText" dxfId="102" priority="42" operator="containsText" text="Research">
       <formula>NOT(ISERROR(SEARCH("Research",A5)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="43" operator="containsText" text="Research">
@@ -25237,131 +25241,131 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="88" priority="36" operator="containsText" text="Data Engineer">
+    <cfRule type="containsText" dxfId="101" priority="36" operator="containsText" text="Data Engineer">
       <formula>NOT(ISERROR(SEARCH("Data Engineer",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="37" operator="containsText" text="Quantitative Analysis">
+    <cfRule type="containsText" dxfId="100" priority="37" operator="containsText" text="Quantitative Analysis">
       <formula>NOT(ISERROR(SEARCH("Quantitative Analysis",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="38" operator="containsText" text="Research Scientist">
+    <cfRule type="containsText" dxfId="99" priority="38" operator="containsText" text="Research Scientist">
       <formula>NOT(ISERROR(SEARCH("Research Scientist",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="39" operator="containsText" text="Research &amp; Analytics">
+    <cfRule type="containsText" dxfId="98" priority="39" operator="containsText" text="Research &amp; Analytics">
       <formula>NOT(ISERROR(SEARCH("Research &amp; Analytics",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="40" operator="containsText" text="Research &amp; Development">
+    <cfRule type="containsText" dxfId="97" priority="40" operator="containsText" text="Research &amp; Development">
       <formula>NOT(ISERROR(SEARCH("Research &amp; Development",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="41" operator="containsText" text="Research">
+    <cfRule type="containsText" dxfId="96" priority="41" operator="containsText" text="Research">
       <formula>NOT(ISERROR(SEARCH("Research",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A1495">
-    <cfRule type="containsText" dxfId="82" priority="1" operator="containsText" text="Assistant">
+    <cfRule type="containsText" dxfId="95" priority="1" operator="containsText" text="Assistant">
       <formula>NOT(ISERROR(SEARCH("Assistant",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="2" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="94" priority="2" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="3" operator="containsText" text="Analytics">
+    <cfRule type="containsText" dxfId="93" priority="3" operator="containsText" text="Analytics">
       <formula>NOT(ISERROR(SEARCH("Analytics",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="4" operator="containsText" text="Business Development &amp; Analytics">
+    <cfRule type="containsText" dxfId="92" priority="4" operator="containsText" text="Business Development &amp; Analytics">
       <formula>NOT(ISERROR(SEARCH("Business Development &amp; Analytics",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="5" operator="containsText" text="Data Operations">
+    <cfRule type="containsText" dxfId="91" priority="5" operator="containsText" text="Data Operations">
       <formula>NOT(ISERROR(SEARCH("Data Operations",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="6" operator="containsText" text="Database">
+    <cfRule type="containsText" dxfId="90" priority="6" operator="containsText" text="Database">
       <formula>NOT(ISERROR(SEARCH("Database",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="7" operator="containsText" text="Software Developer">
+    <cfRule type="containsText" dxfId="89" priority="7" operator="containsText" text="Software Developer">
       <formula>NOT(ISERROR(SEARCH("Software Developer",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="8" operator="containsText" text="Software Engineer">
+    <cfRule type="containsText" dxfId="88" priority="8" operator="containsText" text="Software Engineer">
       <formula>NOT(ISERROR(SEARCH("Software Engineer",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="9" operator="containsText" text="Strategies">
+    <cfRule type="containsText" dxfId="87" priority="9" operator="containsText" text="Strategies">
       <formula>NOT(ISERROR(SEARCH("Strategies",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="10" operator="containsText" text="Baseball Operations – Systems">
+    <cfRule type="containsText" dxfId="86" priority="10" operator="containsText" text="Baseball Operations – Systems">
       <formula>NOT(ISERROR(SEARCH("Baseball Operations – Systems",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="11" operator="containsText" text="Analyst">
+    <cfRule type="containsText" dxfId="85" priority="11" operator="containsText" text="Analyst">
       <formula>NOT(ISERROR(SEARCH("Analyst",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="12" operator="containsText" text=" Baseball Developmental Technology">
+    <cfRule type="containsText" dxfId="84" priority="12" operator="containsText" text=" Baseball Developmental Technology">
       <formula>NOT(ISERROR(SEARCH(" Baseball Developmental Technology",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="13" operator="containsText" text="Player Development">
+    <cfRule type="containsText" dxfId="83" priority="13" operator="containsText" text="Player Development">
       <formula>NOT(ISERROR(SEARCH("Player Development",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="14" operator="containsText" text="Pro Analytics">
+    <cfRule type="containsText" dxfId="82" priority="14" operator="containsText" text="Pro Analytics">
       <formula>NOT(ISERROR(SEARCH("Pro Analytics",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="15" operator="containsText" text="Business Intelligience Analyst">
+    <cfRule type="containsText" dxfId="81" priority="15" operator="containsText" text="Business Intelligience Analyst">
       <formula>NOT(ISERROR(SEARCH("Business Intelligience Analyst",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="16" operator="containsText" text="Business Analyst">
+    <cfRule type="containsText" dxfId="80" priority="16" operator="containsText" text="Business Analyst">
       <formula>NOT(ISERROR(SEARCH("Business Analyst",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="17" operator="containsText" text="Baseball Systems">
+    <cfRule type="containsText" dxfId="79" priority="17" operator="containsText" text="Baseball Systems">
       <formula>NOT(ISERROR(SEARCH("Baseball Systems",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="18" operator="containsText" text="R&amp;D">
+    <cfRule type="containsText" dxfId="78" priority="18" operator="containsText" text="R&amp;D">
       <formula>NOT(ISERROR(SEARCH("R&amp;D",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="19" operator="containsText" text="Pitching Analytics">
+    <cfRule type="containsText" dxfId="77" priority="19" operator="containsText" text="Pitching Analytics">
       <formula>NOT(ISERROR(SEARCH("Pitching Analytics",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="20" operator="containsText" text="Pitching Strategist">
+    <cfRule type="containsText" dxfId="76" priority="20" operator="containsText" text="Pitching Strategist">
       <formula>NOT(ISERROR(SEARCH("Pitching Strategist",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="21" operator="containsText" text="Assistant">
+    <cfRule type="containsText" dxfId="75" priority="21" operator="containsText" text="Assistant">
       <formula>NOT(ISERROR(SEARCH("Assistant",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="23" operator="containsText" text="Baseball Operations Fellow">
+    <cfRule type="containsText" dxfId="74" priority="23" operator="containsText" text="Baseball Operations Fellow">
       <formula>NOT(ISERROR(SEARCH("Baseball Operations Fellow",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="24" operator="containsText" text="Baseball Operations Analyst">
+    <cfRule type="containsText" dxfId="73" priority="24" operator="containsText" text="Baseball Operations Analyst">
       <formula>NOT(ISERROR(SEARCH("Baseball Operations Analyst",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="25" operator="containsText" text="Strategy">
+    <cfRule type="containsText" dxfId="72" priority="25" operator="containsText" text="Strategy">
       <formula>NOT(ISERROR(SEARCH("Strategy",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="26" operator="containsText" text="Business Strategy">
+    <cfRule type="containsText" dxfId="71" priority="26" operator="containsText" text="Business Strategy">
       <formula>NOT(ISERROR(SEARCH("Business Strategy",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="27" operator="containsText" text="Baseball Analytics">
+    <cfRule type="containsText" dxfId="70" priority="27" operator="containsText" text="Baseball Analytics">
       <formula>NOT(ISERROR(SEARCH("Baseball Analytics",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="28" operator="containsText" text="Business Analytics">
+    <cfRule type="containsText" dxfId="69" priority="28" operator="containsText" text="Business Analytics">
       <formula>NOT(ISERROR(SEARCH("Business Analytics",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="29" operator="containsText" text="Business Insights">
+    <cfRule type="containsText" dxfId="68" priority="29" operator="containsText" text="Business Insights">
       <formula>NOT(ISERROR(SEARCH("Business Insights",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="30" operator="containsText" text="Business Intelligence">
+    <cfRule type="containsText" dxfId="67" priority="30" operator="containsText" text="Business Intelligence">
       <formula>NOT(ISERROR(SEARCH("Business Intelligence",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="31" operator="containsText" text="Baseball System Developer">
+    <cfRule type="containsText" dxfId="66" priority="31" operator="containsText" text="Baseball System Developer">
       <formula>NOT(ISERROR(SEARCH("Baseball System Developer",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="32" operator="containsText" text="Software Engineer">
+    <cfRule type="containsText" dxfId="65" priority="32" operator="containsText" text="Software Engineer">
       <formula>NOT(ISERROR(SEARCH("Software Engineer",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="33" operator="containsText" text="DevOps">
+    <cfRule type="containsText" dxfId="64" priority="33" operator="containsText" text="DevOps">
       <formula>NOT(ISERROR(SEARCH("DevOps",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="34" operator="containsText" text="Data Quality Assurance">
+    <cfRule type="containsText" dxfId="63" priority="34" operator="containsText" text="Data Quality Assurance">
       <formula>NOT(ISERROR(SEARCH("Data Quality Assurance",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="35" operator="containsText" text="Data Scientist">
+    <cfRule type="containsText" dxfId="62" priority="35" operator="containsText" text="Data Scientist">
       <formula>NOT(ISERROR(SEARCH("Data Scientist",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A328">
-    <cfRule type="containsText" dxfId="48" priority="22" operator="containsText" text="Player Development">
+    <cfRule type="containsText" dxfId="61" priority="22" operator="containsText" text="Player Development">
       <formula>NOT(ISERROR(SEARCH("Player Development",A328)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31387,27 +31391,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="containsText" dxfId="47" priority="119" operator="containsText" text="Data Engineer">
+    <cfRule type="containsText" dxfId="59" priority="119" operator="containsText" text="Data Engineer">
       <formula>NOT(ISERROR(SEARCH("Data Engineer",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="120" operator="containsText" text="Quantitative Analysis">
+    <cfRule type="containsText" dxfId="58" priority="120" operator="containsText" text="Quantitative Analysis">
       <formula>NOT(ISERROR(SEARCH("Quantitative Analysis",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="121" operator="containsText" text="Research Scientist">
+    <cfRule type="containsText" dxfId="57" priority="121" operator="containsText" text="Research Scientist">
       <formula>NOT(ISERROR(SEARCH("Research Scientist",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="122" operator="containsText" text="Research &amp; Analytics">
+    <cfRule type="containsText" dxfId="56" priority="122" operator="containsText" text="Research &amp; Analytics">
       <formula>NOT(ISERROR(SEARCH("Research &amp; Analytics",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="123" operator="containsText" text="Research &amp; Development">
+    <cfRule type="containsText" dxfId="55" priority="123" operator="containsText" text="Research &amp; Development">
       <formula>NOT(ISERROR(SEARCH("Research &amp; Development",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="124" operator="containsText" text="Research">
+    <cfRule type="containsText" dxfId="54" priority="124" operator="containsText" text="Research">
       <formula>NOT(ISERROR(SEARCH("Research",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:A7">
-    <cfRule type="containsText" dxfId="41" priority="42" operator="containsText" text="Research">
+    <cfRule type="containsText" dxfId="53" priority="42" operator="containsText" text="Research">
       <formula>NOT(ISERROR(SEARCH("Research",A6)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="43" operator="containsText" text="Research">
@@ -31415,131 +31419,131 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A504">
-    <cfRule type="containsText" dxfId="40" priority="36" operator="containsText" text="Data Engineer">
+    <cfRule type="containsText" dxfId="52" priority="36" operator="containsText" text="Data Engineer">
       <formula>NOT(ISERROR(SEARCH("Data Engineer",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="Quantitative Analysis">
+    <cfRule type="containsText" dxfId="51" priority="37" operator="containsText" text="Quantitative Analysis">
       <formula>NOT(ISERROR(SEARCH("Quantitative Analysis",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="Research Scientist">
+    <cfRule type="containsText" dxfId="50" priority="38" operator="containsText" text="Research Scientist">
       <formula>NOT(ISERROR(SEARCH("Research Scientist",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="Research &amp; Analytics">
+    <cfRule type="containsText" dxfId="49" priority="39" operator="containsText" text="Research &amp; Analytics">
       <formula>NOT(ISERROR(SEARCH("Research &amp; Analytics",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="Research &amp; Development">
+    <cfRule type="containsText" dxfId="48" priority="40" operator="containsText" text="Research &amp; Development">
       <formula>NOT(ISERROR(SEARCH("Research &amp; Development",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="41" operator="containsText" text="Research">
+    <cfRule type="containsText" dxfId="47" priority="41" operator="containsText" text="Research">
       <formula>NOT(ISERROR(SEARCH("Research",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:A504">
-    <cfRule type="containsText" dxfId="34" priority="1" operator="containsText" text="Assistant">
+    <cfRule type="containsText" dxfId="46" priority="1" operator="containsText" text="Assistant">
       <formula>NOT(ISERROR(SEARCH("Assistant",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="2" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="45" priority="2" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="3" operator="containsText" text="Analytics">
+    <cfRule type="containsText" dxfId="44" priority="3" operator="containsText" text="Analytics">
       <formula>NOT(ISERROR(SEARCH("Analytics",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="4" operator="containsText" text="Business Development &amp; Analytics">
+    <cfRule type="containsText" dxfId="43" priority="4" operator="containsText" text="Business Development &amp; Analytics">
       <formula>NOT(ISERROR(SEARCH("Business Development &amp; Analytics",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="5" operator="containsText" text="Data Operations">
+    <cfRule type="containsText" dxfId="42" priority="5" operator="containsText" text="Data Operations">
       <formula>NOT(ISERROR(SEARCH("Data Operations",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="6" operator="containsText" text="Database">
+    <cfRule type="containsText" dxfId="41" priority="6" operator="containsText" text="Database">
       <formula>NOT(ISERROR(SEARCH("Database",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="7" operator="containsText" text="Software Developer">
+    <cfRule type="containsText" dxfId="40" priority="7" operator="containsText" text="Software Developer">
       <formula>NOT(ISERROR(SEARCH("Software Developer",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="Software Engineer">
+    <cfRule type="containsText" dxfId="39" priority="8" operator="containsText" text="Software Engineer">
       <formula>NOT(ISERROR(SEARCH("Software Engineer",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="9" operator="containsText" text="Strategies">
+    <cfRule type="containsText" dxfId="38" priority="9" operator="containsText" text="Strategies">
       <formula>NOT(ISERROR(SEARCH("Strategies",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="10" operator="containsText" text="Baseball Operations – Systems">
+    <cfRule type="containsText" dxfId="37" priority="10" operator="containsText" text="Baseball Operations – Systems">
       <formula>NOT(ISERROR(SEARCH("Baseball Operations – Systems",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="11" operator="containsText" text="Analyst">
+    <cfRule type="containsText" dxfId="36" priority="11" operator="containsText" text="Analyst">
       <formula>NOT(ISERROR(SEARCH("Analyst",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="12" operator="containsText" text=" Baseball Developmental Technology">
+    <cfRule type="containsText" dxfId="35" priority="12" operator="containsText" text=" Baseball Developmental Technology">
       <formula>NOT(ISERROR(SEARCH(" Baseball Developmental Technology",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="13" operator="containsText" text="Player Development">
+    <cfRule type="containsText" dxfId="34" priority="13" operator="containsText" text="Player Development">
       <formula>NOT(ISERROR(SEARCH("Player Development",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="14" operator="containsText" text="Pro Analytics">
+    <cfRule type="containsText" dxfId="33" priority="14" operator="containsText" text="Pro Analytics">
       <formula>NOT(ISERROR(SEARCH("Pro Analytics",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="Business Intelligience Analyst">
+    <cfRule type="containsText" dxfId="32" priority="15" operator="containsText" text="Business Intelligience Analyst">
       <formula>NOT(ISERROR(SEARCH("Business Intelligience Analyst",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="Business Analyst">
+    <cfRule type="containsText" dxfId="31" priority="16" operator="containsText" text="Business Analyst">
       <formula>NOT(ISERROR(SEARCH("Business Analyst",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="Baseball Systems">
+    <cfRule type="containsText" dxfId="30" priority="17" operator="containsText" text="Baseball Systems">
       <formula>NOT(ISERROR(SEARCH("Baseball Systems",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="R&amp;D">
+    <cfRule type="containsText" dxfId="29" priority="18" operator="containsText" text="R&amp;D">
       <formula>NOT(ISERROR(SEARCH("R&amp;D",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="Pitching Analytics">
+    <cfRule type="containsText" dxfId="28" priority="19" operator="containsText" text="Pitching Analytics">
       <formula>NOT(ISERROR(SEARCH("Pitching Analytics",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="Pitching Strategist">
+    <cfRule type="containsText" dxfId="27" priority="20" operator="containsText" text="Pitching Strategist">
       <formula>NOT(ISERROR(SEARCH("Pitching Strategist",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="21" operator="containsText" text="Assistant">
+    <cfRule type="containsText" dxfId="26" priority="21" operator="containsText" text="Assistant">
       <formula>NOT(ISERROR(SEARCH("Assistant",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="Baseball Operations Fellow">
+    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="Baseball Operations Fellow">
       <formula>NOT(ISERROR(SEARCH("Baseball Operations Fellow",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="24" operator="containsText" text="Baseball Operations Analyst">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="Baseball Operations Analyst">
       <formula>NOT(ISERROR(SEARCH("Baseball Operations Analyst",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="25" operator="containsText" text="Strategy">
+    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="Strategy">
       <formula>NOT(ISERROR(SEARCH("Strategy",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="26" operator="containsText" text="Business Strategy">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="Business Strategy">
       <formula>NOT(ISERROR(SEARCH("Business Strategy",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="27" operator="containsText" text="Baseball Analytics">
+    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="Baseball Analytics">
       <formula>NOT(ISERROR(SEARCH("Baseball Analytics",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="28" operator="containsText" text="Business Analytics">
+    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="Business Analytics">
       <formula>NOT(ISERROR(SEARCH("Business Analytics",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="29" operator="containsText" text="Business Insights">
+    <cfRule type="containsText" dxfId="19" priority="29" operator="containsText" text="Business Insights">
       <formula>NOT(ISERROR(SEARCH("Business Insights",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="30" operator="containsText" text="Business Intelligence">
+    <cfRule type="containsText" dxfId="18" priority="30" operator="containsText" text="Business Intelligence">
       <formula>NOT(ISERROR(SEARCH("Business Intelligence",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="31" operator="containsText" text="Baseball System Developer">
+    <cfRule type="containsText" dxfId="17" priority="31" operator="containsText" text="Baseball System Developer">
       <formula>NOT(ISERROR(SEARCH("Baseball System Developer",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="32" operator="containsText" text="Software Engineer">
+    <cfRule type="containsText" dxfId="16" priority="32" operator="containsText" text="Software Engineer">
       <formula>NOT(ISERROR(SEARCH("Software Engineer",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="33" operator="containsText" text="DevOps">
+    <cfRule type="containsText" dxfId="15" priority="33" operator="containsText" text="DevOps">
       <formula>NOT(ISERROR(SEARCH("DevOps",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="34" operator="containsText" text="Data Quality Assurance">
+    <cfRule type="containsText" dxfId="14" priority="34" operator="containsText" text="Data Quality Assurance">
       <formula>NOT(ISERROR(SEARCH("Data Quality Assurance",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="35" operator="containsText" text="Data Scientist">
+    <cfRule type="containsText" dxfId="13" priority="35" operator="containsText" text="Data Scientist">
       <formula>NOT(ISERROR(SEARCH("Data Scientist",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A329">
-    <cfRule type="containsText" dxfId="0" priority="22" operator="containsText" text="Player Development">
+    <cfRule type="containsText" dxfId="12" priority="22" operator="containsText" text="Player Development">
       <formula>NOT(ISERROR(SEARCH("Player Development",A329)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31562,7 +31566,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31584,156 +31588,156 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>716</v>
+        <v>1682</v>
       </c>
       <c r="B2" t="s">
-        <v>2470</v>
+        <v>2477</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>431</v>
+        <v>702</v>
       </c>
       <c r="B3" t="s">
-        <v>2458</v>
+        <v>2467</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>472</v>
+        <v>1125</v>
       </c>
       <c r="B4" t="s">
-        <v>2460</v>
+        <v>2474</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1045</v>
+        <v>345</v>
       </c>
       <c r="B5" t="s">
-        <v>2462</v>
+        <v>2455</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1799</v>
+        <v>1333</v>
       </c>
       <c r="B6" t="s">
-        <v>2463</v>
+        <v>2468</v>
       </c>
       <c r="C6">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1305</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>2475</v>
+        <v>2451</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1800</v>
+        <v>879</v>
       </c>
       <c r="B8" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
       <c r="C8">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>332</v>
+        <v>482</v>
       </c>
       <c r="B9" t="s">
-        <v>2454</v>
+        <v>2461</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>256</v>
+        <v>455</v>
       </c>
       <c r="B10" t="s">
-        <v>2464</v>
+        <v>2459</v>
       </c>
       <c r="C10">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1497</v>
+        <v>798</v>
       </c>
       <c r="B11" t="s">
-        <v>2466</v>
+        <v>2480</v>
       </c>
       <c r="C11">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>573</v>
+        <v>963</v>
       </c>
       <c r="B12" t="s">
-        <v>2478</v>
+        <v>2481</v>
       </c>
       <c r="C12">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1331</v>
+        <v>635</v>
       </c>
       <c r="B13" t="s">
-        <v>2473</v>
+        <v>2453</v>
       </c>
       <c r="C13">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1741</v>
+        <v>797</v>
       </c>
       <c r="B14" t="s">
-        <v>2476</v>
+        <v>2465</v>
       </c>
       <c r="C14">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="B15" t="s">
-        <v>2457</v>
+        <v>2456</v>
       </c>
       <c r="C15">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -31760,162 +31764,163 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>635</v>
+        <v>1331</v>
       </c>
       <c r="B18" t="s">
-        <v>2453</v>
+        <v>2473</v>
       </c>
       <c r="C18">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>797</v>
+        <v>1741</v>
       </c>
       <c r="B19" t="s">
-        <v>2465</v>
+        <v>2476</v>
       </c>
       <c r="C19">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>374</v>
+        <v>390</v>
       </c>
       <c r="B20" t="s">
-        <v>2456</v>
+        <v>2457</v>
       </c>
       <c r="C20">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>798</v>
+        <v>256</v>
       </c>
       <c r="B21" t="s">
-        <v>2480</v>
+        <v>2464</v>
       </c>
       <c r="C21">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>963</v>
+        <v>1497</v>
       </c>
       <c r="B22" t="s">
-        <v>2481</v>
+        <v>2466</v>
       </c>
       <c r="C22">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>482</v>
+        <v>573</v>
       </c>
       <c r="B23" t="s">
-        <v>2461</v>
+        <v>2478</v>
       </c>
       <c r="C23">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>455</v>
+        <v>1800</v>
       </c>
       <c r="B24" t="s">
-        <v>2459</v>
+        <v>2472</v>
       </c>
       <c r="C24">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>332</v>
       </c>
       <c r="B25" t="s">
-        <v>2451</v>
+        <v>2454</v>
       </c>
       <c r="C25">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>879</v>
+        <v>1305</v>
       </c>
       <c r="B26" t="s">
-        <v>2471</v>
+        <v>2475</v>
       </c>
       <c r="C26">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1333</v>
+        <v>1045</v>
       </c>
       <c r="B27" t="s">
-        <v>2468</v>
+        <v>2462</v>
       </c>
       <c r="C27">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>345</v>
+        <v>1799</v>
       </c>
       <c r="B28" t="s">
-        <v>2455</v>
+        <v>2463</v>
       </c>
       <c r="C28">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1125</v>
+        <v>716</v>
       </c>
       <c r="B29" t="s">
-        <v>2474</v>
+        <v>2470</v>
       </c>
       <c r="C29">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>702</v>
+        <v>431</v>
       </c>
       <c r="B30" t="s">
-        <v>2467</v>
+        <v>2458</v>
       </c>
       <c r="C30">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1682</v>
+        <v>472</v>
       </c>
       <c r="B31" t="s">
-        <v>2477</v>
+        <v>2460</v>
       </c>
       <c r="C31">
-        <v>39</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>